<commit_message>
change adress in page ecopromo
</commit_message>
<xml_diff>
--- a/src/assets/files/price.xlsx
+++ b/src/assets/files/price.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="390" windowWidth="18915" windowHeight="11475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>№</t>
   </si>
@@ -97,9 +102,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>5-6</t>
-  </si>
-  <si>
     <t>Газеты</t>
   </si>
   <si>
@@ -173,12 +175,15 @@
   </si>
   <si>
     <t>7</t>
+  </si>
+  <si>
+    <t>6-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,6 +466,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -509,7 +517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +552,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -756,7 +764,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,10 +812,10 @@
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>4</v>
@@ -833,16 +841,16 @@
         <v>4.5</v>
       </c>
       <c r="D4" s="3">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="E4" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>8</v>
@@ -869,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>8</v>
@@ -880,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
@@ -895,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>8</v>
@@ -906,22 +914,22 @@
         <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>5.5</v>
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>8</v>
@@ -932,22 +940,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="E8" s="3">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3">
-        <v>5.5</v>
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>8</v>
@@ -970,10 +978,10 @@
         <v>12</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>8</v>
@@ -996,10 +1004,10 @@
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>8</v>
@@ -1022,10 +1030,10 @@
         <v>7</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>8</v>
@@ -1048,10 +1056,10 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>8</v>
@@ -1114,7 +1122,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>24</v>
@@ -1155,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>8</v>
@@ -1166,7 +1174,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3">
         <v>5</v>
@@ -1181,7 +1189,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>8</v>
@@ -1192,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
@@ -1207,7 +1215,7 @@
         <v>2</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>8</v>
@@ -1218,7 +1226,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
         <v>5</v>
@@ -1233,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>8</v>
@@ -1244,7 +1252,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3">
         <v>1</v>
@@ -1259,7 +1267,7 @@
         <v>1.4</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>8</v>
@@ -1270,7 +1278,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3">
         <v>2</v>
@@ -1285,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>8</v>
@@ -1296,7 +1304,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
@@ -1322,7 +1330,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="11">
         <v>8</v>
@@ -1374,7 +1382,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="11">
         <v>0</v>
@@ -1389,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>8</v>
@@ -1397,7 +1405,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>

</xml_diff>